<commit_message>
Add properties for omitting missing rows and columns
</commit_message>
<xml_diff>
--- a/Assets/Development/TestFiles/EmptyRows.xlsx
+++ b/Assets/Development/TestFiles/EmptyRows.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APLProjects\CarlisleGroup\XL2APL\Assets\Development\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APLProjects\XL2APL\Assets\Development\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F47C975E-F6F2-48DB-9AED-BA18627D442F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52EC303-A93F-4718-AB5A-59DC8A2DAC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{08EB3DB6-F474-4250-A700-6703F8B07C24}"/>
+    <workbookView xWindow="34980" yWindow="-4800" windowWidth="21600" windowHeight="11265" xr2:uid="{08EB3DB6-F474-4250-A700-6703F8B07C24}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,12 +397,12 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -416,7 +416,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11</v>
       </c>
@@ -430,7 +430,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>21</v>
       </c>
@@ -444,7 +444,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>41</v>
       </c>
@@ -458,7 +458,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>61</v>
       </c>
@@ -469,7 +469,7 @@
         <v>63</v>
       </c>
       <c r="E7">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>